<commit_message>
tring to solve Software caused connection abort: socket write error
</commit_message>
<xml_diff>
--- a/autotest/TestData/TestData.xlsx
+++ b/autotest/TestData/TestData.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="6" r:id="rId1"/>
     <sheet name="api" sheetId="2" r:id="rId2"/>
     <sheet name="address" sheetId="8" r:id="rId3"/>
-    <sheet name="buyprocess" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
-    <sheet name="gift" sheetId="9" r:id="rId6"/>
-    <sheet name="quickbuy" sheetId="7" r:id="rId7"/>
-    <sheet name="login" sheetId="12" r:id="rId8"/>
-    <sheet name="giftbackup" sheetId="4" r:id="rId9"/>
-    <sheet name="phonebackup" sheetId="3" r:id="rId10"/>
+    <sheet name="changeArea" sheetId="16" r:id="rId4"/>
+    <sheet name="buyprocess" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
+    <sheet name="gift" sheetId="9" r:id="rId7"/>
+    <sheet name="quickbuy" sheetId="7" r:id="rId8"/>
+    <sheet name="login" sheetId="12" r:id="rId9"/>
+    <sheet name="giftbackup" sheetId="4" r:id="rId10"/>
+    <sheet name="phonebackup" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">api!$B$1:$G$24</definedName>
@@ -70,6 +71,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
+    <author>admin</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0">
@@ -675,12 +677,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="B25" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+东角山：%E4%B8%9C%E8%A7%92%E5%B1%B1
+万科城：%E4%B8%87%E7%A7%91%E5%9F%8E
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="298">
   <si>
     <t>api</t>
   </si>
@@ -6516,10 +6544,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>wx:3.9.6</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>/v3/setting/address</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -6761,10 +6785,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>/ja/user/v4/discovery/cae/search?limit=10&amp;page=1&amp;keyword=</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>application/json</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -6813,9 +6833,6 @@
   <si>
     <t>获取收货地址</t>
     <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <r>
@@ -6924,6 +6941,57 @@
   </si>
   <si>
     <t>老用户在切换小区中定位</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
+  </si>
+  <si>
+    <t>搜索小区</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wx:3.9.8</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v4/discovery/cae/search?limit=10&amp;page=1&amp;keyword=</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v3/od/region/villages/search/东角山?currentRegion=false&amp;latitude=22.54605355&amp;limit=20&amp;longitude=114.02597366&amp;page=1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换小区</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v3/od/zone/lbs/change</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域切换成功</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"自动化测试花园","address":"张大爷的测试","province":"广东省","city":"深圳","latitude":22.410132,"longitude":113.824495,"addressNaviId":18401,"regionId":813395}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"万科城","address":"广东省深圳市龙岗区坂雪岗工业区坂雪岗大道","province":"广东省","city":"深圳","latitude":22.651245,"longitude":114.076476,"addressNaviId":18031,"regionId":2}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"东角山","address":"广东省深圳市南山区","province":"广东省","city":"深圳","latitude":22.408965,"longitude":113.826119,"addressNaviId":18039,"regionId":813395}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>wx:3.9.6</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -6931,7 +6999,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7027,6 +7095,25 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -7074,7 +7161,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7111,11 +7198,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7397,7 +7490,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7409,64 +7502,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
+      <c r="A1" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="3" spans="1:26" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>269</v>
+    <row r="3" spans="1:26" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B5" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.15">
@@ -7477,68 +7570,68 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B9" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B10" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B11" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B12" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="C14" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="C15" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="C16" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C17" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C19" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C20" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -7553,6 +7646,116 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="26.75" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.375" collapsed="1"/>
+    <col min="8" max="8" width="10.875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.625" collapsed="1"/>
+    <col min="13" max="13" width="12" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -8062,16 +8265,17 @@
   <sheetPr filterMode="1">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.75" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="124.75" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.5" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="44.75" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22.875" style="1" customWidth="1" collapsed="1"/>
@@ -8082,7 +8286,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -8100,24 +8304,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -8131,10 +8335,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>8</v>
@@ -8148,7 +8352,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -8159,16 +8363,16 @@
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -8179,19 +8383,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>233</v>
@@ -8199,19 +8403,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -8219,11 +8423,11 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -8238,7 +8442,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -8253,7 +8457,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>7</v>
@@ -8267,7 +8471,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
@@ -8278,13 +8482,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -8298,7 +8502,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>7</v>
@@ -8313,7 +8517,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
@@ -8324,10 +8528,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D15" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>7</v>
@@ -8341,7 +8545,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>7</v>
@@ -8350,12 +8554,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
@@ -8364,13 +8568,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
@@ -8379,13 +8583,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>7</v>
@@ -8394,28 +8598,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>7</v>
@@ -8424,13 +8628,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
@@ -8439,13 +8643,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -8454,13 +8658,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>7</v>
@@ -8468,6 +8672,82 @@
       <c r="F24" s="3" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>290</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D38"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G24">
@@ -8497,8 +8777,8 @@
   <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8522,15 +8802,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>31</v>
@@ -8858,7 +9138,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>31</v>
@@ -9160,6 +9440,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="219.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -9204,7 +9538,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>238</v>
@@ -9224,7 +9558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9237,7 +9571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -9310,7 +9644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -9376,7 +9710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -9405,120 +9739,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="26.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.375" collapsed="1"/>
-    <col min="8" max="8" width="10.875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.625" collapsed="1"/>
-    <col min="13" max="13" width="12" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use testNG 6.9.5 to solve the issue :  java.net.SocketException: Software caused connection abort: socket write error
</commit_message>
<xml_diff>
--- a/autotest/TestData/TestData.xlsx
+++ b/autotest/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="6" r:id="rId1"/>
@@ -708,7 +708,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="304">
   <si>
     <t>api</t>
   </si>
@@ -6835,19 +6835,282 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>业务流</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>业务单元</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>购物流程</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>定位</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类选商品</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增地址</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>购物车</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单确认</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>支付模块</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>支付成功</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>支付失败</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>会员宝支付</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信支付</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消订单</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请售后</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单备注修改</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录模块</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>新用户首页定位</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单模块</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>老用户在切换小区中定位</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
+  </si>
+  <si>
+    <t>搜索小区</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wx:3.9.8</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v4/discovery/cae/search?limit=10&amp;page=1&amp;keyword=</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v3/od/region/villages/search/东角山?currentRegion=false&amp;latitude=22.54605355&amp;limit=20&amp;longitude=114.02597366&amp;page=1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换小区</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v3/od/zone/lbs/change</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域切换成功</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"自动化测试花园","address":"张大爷的测试","province":"广东省","city":"深圳","latitude":22.410132,"longitude":113.824495,"addressNaviId":18401,"regionId":813395}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"万科城","address":"广东省深圳市龙岗区坂雪岗工业区坂雪岗大道","province":"广东省","city":"深圳","latitude":22.651245,"longitude":114.076476,"addressNaviId":18031,"regionId":2}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"name":"东角山","address":"广东省深圳市南山区","province":"广东省","city":"深圳","latitude":22.408965,"longitude":113.826119,"addressNaviId":18039,"regionId":813395}</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>wx:3.9.6</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取小区列表</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ja/user/v3/od/my/regions</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>运行用例时，需要关闭excel表格
+      <t>1.环境配置</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Software version:
+TestNG </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6.9.5.201505251947</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Eclipse Version: Neon.3 Release (4.7.0), Build id: 20170620-1800
+JRE: 1.8.0
+Other jars：please refer to pom.xml
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.用例编写步骤</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+a.在excel表格api sheet添加接口信息
+b.在ApiEnum.java 添加接口信息
+c.如果有测试数据，在excel表格添加相应sheet
+d.如果有测试数据，在FileEnum.java添加数据sheet常量
+e.如果有测试数据，在ApiTestDataPro.java添加数据提供@DataProvider
+f.在ApiTest.java添加测试用例@Test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.excel数据说明</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 api sheet：放置接口信息
-address sheet: 放置新增地址接口测试所需数据，包括手机号码段验证，地址各数据验证（特殊字符，空字符，空，长度，字母等）</t>
+address sheet: 放置新增地址接口测试所需数据，包括手机号码段验证，地址各数据验证（特殊字符，空字符，空，长度，字母等）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.other issue</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+a. testNG version bug: https://github.com/cbeust/testng-eclipse/issues/91(java.net.SocketException: Software caused connection abort: socket write error)
+b. 运行用例时，需要关闭excel表格</t>
     </r>
     <r>
       <rPr>
@@ -6864,142 +7127,27 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>业务流</t>
+    <t>切换不同社区</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>业务单元</t>
+    <t>切换相同社区不同花园</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>购物流程</t>
+    <t>切换到中央仓库</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>定位</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类选商品</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增地址</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>购物车</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单确认</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>支付模块</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>支付成功</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>支付失败</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>会员宝支付</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>微信支付</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>取消订单</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>申请售后</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单备注修改</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>登录模块</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>新用户首页定位</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单模块</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>老用户在切换小区中定位</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
-  </si>
-  <si>
-    <t>搜索小区</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wx:3.9.8</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ja/user/v4/discovery/cae/search?limit=10&amp;page=1&amp;keyword=</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ja/user/v3/od/region/villages/search/东角山?currentRegion=false&amp;latitude=22.54605355&amp;limit=20&amp;longitude=114.02597366&amp;page=1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>fea95893-4c02-4f5f-9b38-d6292d955f41</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>切换小区</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ja/user/v3/od/zone/lbs/change</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域切换成功</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"name":"自动化测试花园","address":"张大爷的测试","province":"广东省","city":"深圳","latitude":22.410132,"longitude":113.824495,"addressNaviId":18401,"regionId":813395}</t>
+    <t>{"name":"中央仓库","address":"","province":"广东省","city":"深圳市","latitude":0,"longitude":0,"addressNaviId":0,"regionId":4}</t>
     <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"name":"万科城","address":"广东省深圳市龙岗区坂雪岗工业区坂雪岗大道","province":"广东省","city":"深圳","latitude":22.651245,"longitude":114.076476,"addressNaviId":18031,"regionId":2}</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"name":"东角山","address":"广东省深圳市南山区","province":"广东省","city":"深圳","latitude":22.408965,"longitude":113.826119,"addressNaviId":18039,"regionId":813395}</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>wx:3.9.6</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7114,6 +7262,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -7161,7 +7318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7201,14 +7358,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7488,10 +7648,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7501,76 +7661,87 @@
     <col min="3" max="3" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-    </row>
-    <row r="2" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="1" spans="1:26" ht="322.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+    </row>
+    <row r="2" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="10">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>265</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B5" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B5" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B9" s="11" t="s">
-        <v>270</v>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.15">
@@ -7580,35 +7751,35 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B11" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B12" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B14" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>273</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="C14" s="11" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="C15" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="C16" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
@@ -7617,21 +7788,26 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B18" s="11" t="s">
-        <v>283</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="11" t="s">
+        <v>282</v>
+      </c>
       <c r="C19" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C20" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C21" s="11" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -8268,8 +8444,8 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8318,7 +8494,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>241</v>
@@ -8335,7 +8511,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>243</v>
@@ -8352,7 +8528,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -8372,7 +8548,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -8392,7 +8568,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>257</v>
@@ -8412,7 +8588,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>254</v>
@@ -8427,7 +8603,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -8442,7 +8618,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -8457,7 +8633,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>7</v>
@@ -8471,7 +8647,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
@@ -8488,7 +8664,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -8502,7 +8678,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>7</v>
@@ -8517,7 +8693,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
@@ -8531,7 +8707,7 @@
         <v>250</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>7</v>
@@ -8545,7 +8721,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>7</v>
@@ -8559,7 +8735,7 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
@@ -8574,7 +8750,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
@@ -8589,7 +8765,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>7</v>
@@ -8604,13 +8780,13 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -8619,7 +8795,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>7</v>
@@ -8634,7 +8810,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
@@ -8649,7 +8825,7 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -8660,11 +8836,11 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>7</v>
@@ -8675,46 +8851,63 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>288</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D27"/>
+      <c r="A27" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D28"/>
@@ -9441,15 +9634,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="219.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="181.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
@@ -9463,27 +9657,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
-        <v>294</v>
+      <c r="A2" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>295</v>
+      <c r="A3" s="14" t="s">
+        <v>303</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try maven: use command: mvn install
</commit_message>
<xml_diff>
--- a/autotest/TestData/TestData.xlsx
+++ b/autotest/TestData/TestData.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\eclipse-workspace\autoTest\autotest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowHeight="10350" windowWidth="23895" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Note" sheetId="6" r:id="rId1"/>
-    <sheet name="api" sheetId="2" r:id="rId2"/>
-    <sheet name="address" sheetId="8" r:id="rId3"/>
-    <sheet name="changeArea" sheetId="16" r:id="rId4"/>
-    <sheet name="buyprocess" sheetId="11" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
-    <sheet name="gift" sheetId="9" r:id="rId7"/>
-    <sheet name="quickbuy" sheetId="7" r:id="rId8"/>
-    <sheet name="login" sheetId="12" r:id="rId9"/>
-    <sheet name="giftbackup" sheetId="4" r:id="rId10"/>
-    <sheet name="phonebackup" sheetId="3" r:id="rId11"/>
+    <sheet name="Note" r:id="rId1" sheetId="6"/>
+    <sheet name="api" r:id="rId2" sheetId="2"/>
+    <sheet name="address" r:id="rId3" sheetId="8"/>
+    <sheet name="changeArea" r:id="rId4" sheetId="16"/>
+    <sheet name="buyprocess" r:id="rId5" sheetId="11"/>
+    <sheet name="Sheet1" r:id="rId6" sheetId="15"/>
+    <sheet name="gift" r:id="rId7" sheetId="9"/>
+    <sheet name="quickbuy" r:id="rId8" sheetId="7"/>
+    <sheet name="login" r:id="rId9" sheetId="12"/>
+    <sheet name="giftbackup" r:id="rId10" sheetId="4"/>
+    <sheet name="phonebackup" r:id="rId11" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">api!$B$1:$G$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">api!$B$1:$G$24</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -37,7 +37,7 @@
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="E1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="G1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -293,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -437,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -461,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -485,7 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B17" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B18" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -533,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -557,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B20" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -581,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B21" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B22" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -629,7 +629,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B23" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -653,7 +653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B24" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -677,7 +677,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="1" shapeId="0">
+    <comment authorId="1" ref="B25" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -708,7 +708,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="306">
   <si>
     <t>api</t>
   </si>
@@ -7142,11 +7142,18 @@
     <t>{"name":"中央仓库","address":"","province":"广东省","city":"深圳市","latitude":0,"longitude":0,"addressNaviId":0,"regionId":4}</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
+  <si>
+    <t>40fa6da3-721d-4a94-9544-ad029fa7df6d</t>
+  </si>
+  <si>
+    <t>9952425f-1479-4607-9793-7e946b03fdb1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7314,68 +7321,68 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="2" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -7392,10 +7399,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -7559,21 +7566,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -7590,7 +7597,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -7644,11 +7651,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:Z1"/>
@@ -7656,12 +7663,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="322.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="322.5" r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>299</v>
       </c>
@@ -7691,12 +7698,12 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.15">
+    <row customFormat="1" r="2" s="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customFormat="1" customHeight="1" ht="21.75" r="3" s="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>264</v>
       </c>
@@ -7815,15 +7822,15 @@
     <mergeCell ref="A1:Z1"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
@@ -7831,14 +7838,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.375" collapsed="1"/>
-    <col min="8" max="8" width="10.875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.625" collapsed="1"/>
-    <col min="13" max="13" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="26.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="24.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="20.625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="29.375" collapsed="true"/>
+    <col min="7" max="7" width="10.375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="10.875" collapsed="true"/>
+    <col min="9" max="9" width="12.625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -7927,13 +7934,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
@@ -7941,9 +7948,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="64.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="64.125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -8056,7 +8063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="12" r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -8432,35 +8439,35 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
   <sheetPr filterMode="1">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A27" pane="bottomLeft" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="124.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="11.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="124.75" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="20.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.75" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>259</v>
       </c>
@@ -8494,7 +8501,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>241</v>
@@ -8511,7 +8518,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>243</v>
@@ -8528,7 +8535,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -8537,7 +8544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="18" r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>262</v>
       </c>
@@ -8548,7 +8555,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -8568,7 +8575,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>257</v>
@@ -8588,7 +8595,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>254</v>
@@ -8603,7 +8610,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -8618,7 +8625,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -8633,7 +8640,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>7</v>
@@ -8647,7 +8654,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
@@ -8664,7 +8671,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -8678,7 +8685,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>7</v>
@@ -8693,7 +8700,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
@@ -8707,7 +8714,7 @@
         <v>250</v>
       </c>
       <c r="D15" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>7</v>
@@ -8721,7 +8728,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>7</v>
@@ -8735,7 +8742,7 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
@@ -8750,7 +8757,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
@@ -8765,7 +8772,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>7</v>
@@ -8780,7 +8787,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
@@ -8795,7 +8802,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>7</v>
@@ -8810,7 +8817,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
@@ -8825,7 +8832,7 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -8840,7 +8847,7 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>7</v>
@@ -8860,7 +8867,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
@@ -8879,8 +8886,8 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>289</v>
+      <c r="D26" t="s">
+        <v>305</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>7</v>
@@ -8899,8 +8906,8 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>289</v>
+      <c r="D27" t="s">
+        <v>305</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
@@ -8910,37 +8917,59 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D28"/>
+      <c r="D28" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D29"/>
+      <c r="D29" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D30"/>
+      <c r="D30" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D31"/>
+      <c r="D31" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D32"/>
+      <c r="D32" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D33"/>
+      <c r="D33" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D34"/>
+      <c r="D34" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D35"/>
+      <c r="D35" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D36"/>
+      <c r="D36" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D37"/>
+      <c r="D37" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D38"/>
+      <c r="D38" t="s">
+        <v>305</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:G24">
@@ -8952,37 +8981,37 @@
   </autoFilter>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C981">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C981" type="list">
       <formula1>"get,post,put,delete,head,connect,options,trace,patch,move,copy,link,unlink,wrapped,extension-mothed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E1:E1048576" type="list">
       <formula1>"application/json,application/x-www-form-urlencoded,multipart/form-data,application/xhtml+xml,application/xml,application/atom+xml,application/pdf,application/msword,application/octet-stream,text/html,text/plain,text/xml,image/gif, image/jpeg, image/png"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="255.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="9" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="9" style="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="255.125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="29.375" collapsed="true"/>
+    <col min="3" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="10.875" collapsed="true"/>
+    <col min="7" max="10" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9369,7 +9398,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15" r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>211</v>
       </c>
@@ -9627,25 +9656,25 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A14" pane="bottomLeft" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="181.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="181.125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9690,14 +9719,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -9705,13 +9734,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="102.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="9" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="9" style="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="102.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="29.375" collapsed="true"/>
+    <col min="3" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="10.875" collapsed="true"/>
+    <col min="7" max="10" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9756,12 +9785,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9769,13 +9798,13 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -9783,13 +9812,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="48.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="9" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="9" style="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="48.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="29.375" collapsed="true"/>
+    <col min="3" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="10.875" collapsed="true"/>
+    <col min="7" max="10" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9842,13 +9871,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
@@ -9856,13 +9885,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="9" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="9" style="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="70.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="45.375" collapsed="true"/>
+    <col min="3" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="10.875" collapsed="true"/>
+    <col min="7" max="10" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9907,14 +9936,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -9922,13 +9951,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="57.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="9" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="9" style="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="57.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="29.375" collapsed="true"/>
+    <col min="3" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="10.875" collapsed="true"/>
+    <col min="7" max="10" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -9949,6 +9978,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>